<commit_message>
Updated tests with grouping and added Faker serialization logic
</commit_message>
<xml_diff>
--- a/testdata/apiData.xlsx
+++ b/testdata/apiData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9EF78B1D-E16C-4FF5-BD7E-F59708C51BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5DAD1AD4-0D6B-4588-BC4C-4974EC56FAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A459B23-67B7-4DC2-AF59-1602C15F0373}"/>
   </bookViews>
@@ -16,15 +16,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -56,9 +47,6 @@
     <t>jyothi</t>
   </si>
   <si>
-    <t>jyothia</t>
-  </si>
-  <si>
     <t>jypthia</t>
   </si>
   <si>
@@ -75,6 +63,9 @@
   </si>
   <si>
     <t>jyothi1234</t>
+  </si>
+  <si>
+    <t>jyothiaaS</t>
   </si>
 </sst>
 </file>
@@ -440,7 +431,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,19 +472,19 @@
         <v>111111</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>4567888888</v>
@@ -504,19 +495,19 @@
         <v>6754895</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>778885778677</v>

</xml_diff>